<commit_message>
update by excel of states, regions, voltages, element_types, conductor_types over
</commit_message>
<xml_diff>
--- a/database_design/db_exp.xlsx
+++ b/database_design/db_exp.xlsx
@@ -9,20 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="regions" sheetId="7" r:id="rId1"/>
     <sheet name="states" sheetId="8" r:id="rId2"/>
     <sheet name="voltage_levels" sheetId="5" r:id="rId3"/>
-    <sheet name="owners" sheetId="2" r:id="rId4"/>
-    <sheet name="element_types" sheetId="4" r:id="rId5"/>
-    <sheet name="substations" sheetId="1" r:id="rId6"/>
-    <sheet name="conductor_types" sheetId="3" r:id="rId7"/>
+    <sheet name="element_types" sheetId="4" r:id="rId4"/>
+    <sheet name="conductor_types" sheetId="3" r:id="rId5"/>
+    <sheet name="owners" sheetId="2" r:id="rId6"/>
+    <sheet name="substations" sheetId="1" r:id="rId7"/>
     <sheet name="400kVLines" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">owners!$A$1:$D$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">owners!$A$1:$D$83</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="306">
   <si>
     <t>ACBIL</t>
   </si>
@@ -946,6 +946,12 @@
   </si>
   <si>
     <t xml:space="preserve">Vadodora-PS </t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>not yet</t>
   </si>
 </sst>
 </file>
@@ -1279,7 +1285,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1781,986 +1787,152 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E83"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>281</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>286</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>179</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>273</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>284</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>283</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>282</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>168</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>193</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>192</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>186</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>279</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>157</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>172</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" s="4"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>148</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>162</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>280</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" s="4"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>189</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" s="4"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33" s="4"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>180</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>174</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>141</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>169</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>45</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>274</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>275</v>
-      </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40" s="4"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>270</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>181</v>
-      </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43" t="s">
-        <v>61</v>
-      </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44" t="s">
-        <v>171</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" s="4"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" t="s">
-        <v>194</v>
-      </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45" s="4"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46" t="s">
-        <v>140</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>191</v>
-      </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47" s="4"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48" t="s">
-        <v>68</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48" s="4"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49" t="s">
-        <v>269</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49" s="4"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="B50" t="s">
-        <v>156</v>
-      </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50" s="4"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51" t="s">
-        <v>166</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51" s="4"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52" t="s">
-        <v>155</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52" s="4"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>127</v>
-      </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53" s="4"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>184</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="E54" s="4"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>195</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="E55" s="4"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56" t="s">
-        <v>72</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="B57" t="s">
-        <v>176</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="B58" t="s">
-        <v>285</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="B59" t="s">
-        <v>272</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60" t="s">
-        <v>187</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61" t="s">
-        <v>276</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62" t="s">
-        <v>287</v>
-      </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63" t="s">
-        <v>85</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="B64" t="s">
-        <v>86</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="B65" t="s">
-        <v>182</v>
-      </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="B66" t="s">
-        <v>289</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>175</v>
-      </c>
-      <c r="D67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68" t="s">
-        <v>93</v>
-      </c>
-      <c r="D68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="B69" t="s">
-        <v>277</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="B70" t="s">
-        <v>190</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71" t="s">
-        <v>271</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="B72" t="s">
-        <v>163</v>
-      </c>
-      <c r="D72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73" t="s">
-        <v>278</v>
-      </c>
-      <c r="D73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74" t="s">
-        <v>183</v>
-      </c>
-      <c r="D74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="B75" t="s">
-        <v>170</v>
-      </c>
-      <c r="D75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>75</v>
-      </c>
-      <c r="B76" t="s">
-        <v>101</v>
-      </c>
-      <c r="D76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="B77" t="s">
-        <v>288</v>
-      </c>
-      <c r="D77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78" t="s">
-        <v>188</v>
-      </c>
-      <c r="D78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79" t="s">
-        <v>178</v>
-      </c>
-      <c r="D79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>79</v>
-      </c>
-      <c r="B80" t="s">
-        <v>173</v>
-      </c>
-      <c r="D80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>80</v>
-      </c>
-      <c r="B81" t="s">
-        <v>160</v>
-      </c>
-      <c r="D81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>81</v>
-      </c>
-      <c r="B82" t="s">
-        <v>154</v>
-      </c>
-      <c r="D82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>82</v>
-      </c>
-      <c r="B83" t="s">
-        <v>161</v>
-      </c>
-      <c r="D83">
-        <v>1</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2770,96 +1942,63 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>216</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2868,6 +2007,1242 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D3" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D4" t="s">
+        <v>222</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" t="s">
+        <v>305</v>
+      </c>
+      <c r="D5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" t="s">
+        <v>305</v>
+      </c>
+      <c r="D7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" t="s">
+        <v>305</v>
+      </c>
+      <c r="D8" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" t="s">
+        <v>305</v>
+      </c>
+      <c r="D9" t="s">
+        <v>222</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>305</v>
+      </c>
+      <c r="D10" t="s">
+        <v>222</v>
+      </c>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>281</v>
+      </c>
+      <c r="C11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D11" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12" t="s">
+        <v>305</v>
+      </c>
+      <c r="D12" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>286</v>
+      </c>
+      <c r="C14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D14" t="s">
+        <v>222</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" t="s">
+        <v>305</v>
+      </c>
+      <c r="D15" t="s">
+        <v>222</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>179</v>
+      </c>
+      <c r="C16" t="s">
+        <v>305</v>
+      </c>
+      <c r="D16" t="s">
+        <v>222</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>273</v>
+      </c>
+      <c r="C17" t="s">
+        <v>305</v>
+      </c>
+      <c r="D17" t="s">
+        <v>222</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>284</v>
+      </c>
+      <c r="C18" t="s">
+        <v>305</v>
+      </c>
+      <c r="D18" t="s">
+        <v>222</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>283</v>
+      </c>
+      <c r="C19" t="s">
+        <v>305</v>
+      </c>
+      <c r="D19" t="s">
+        <v>222</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>282</v>
+      </c>
+      <c r="C20" t="s">
+        <v>305</v>
+      </c>
+      <c r="D20" t="s">
+        <v>222</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C21" t="s">
+        <v>305</v>
+      </c>
+      <c r="D21" t="s">
+        <v>222</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" t="s">
+        <v>305</v>
+      </c>
+      <c r="D22" t="s">
+        <v>222</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>192</v>
+      </c>
+      <c r="C23" t="s">
+        <v>305</v>
+      </c>
+      <c r="D23" t="s">
+        <v>222</v>
+      </c>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>186</v>
+      </c>
+      <c r="C24" t="s">
+        <v>305</v>
+      </c>
+      <c r="D24" t="s">
+        <v>222</v>
+      </c>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>279</v>
+      </c>
+      <c r="C25" t="s">
+        <v>305</v>
+      </c>
+      <c r="D25" t="s">
+        <v>222</v>
+      </c>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>157</v>
+      </c>
+      <c r="C26" t="s">
+        <v>305</v>
+      </c>
+      <c r="D26" t="s">
+        <v>222</v>
+      </c>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>172</v>
+      </c>
+      <c r="C27" t="s">
+        <v>305</v>
+      </c>
+      <c r="D27" t="s">
+        <v>222</v>
+      </c>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" t="s">
+        <v>305</v>
+      </c>
+      <c r="D28" t="s">
+        <v>222</v>
+      </c>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" t="s">
+        <v>305</v>
+      </c>
+      <c r="D29" t="s">
+        <v>222</v>
+      </c>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>305</v>
+      </c>
+      <c r="D30" t="s">
+        <v>222</v>
+      </c>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>280</v>
+      </c>
+      <c r="C31" t="s">
+        <v>305</v>
+      </c>
+      <c r="D31" t="s">
+        <v>222</v>
+      </c>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32" t="s">
+        <v>305</v>
+      </c>
+      <c r="D32" t="s">
+        <v>222</v>
+      </c>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" t="s">
+        <v>305</v>
+      </c>
+      <c r="D33" t="s">
+        <v>222</v>
+      </c>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C34" t="s">
+        <v>305</v>
+      </c>
+      <c r="D34" t="s">
+        <v>222</v>
+      </c>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" t="s">
+        <v>305</v>
+      </c>
+      <c r="D35" t="s">
+        <v>222</v>
+      </c>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" t="s">
+        <v>305</v>
+      </c>
+      <c r="D36" t="s">
+        <v>222</v>
+      </c>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>169</v>
+      </c>
+      <c r="C37" t="s">
+        <v>305</v>
+      </c>
+      <c r="D37" t="s">
+        <v>222</v>
+      </c>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" t="s">
+        <v>305</v>
+      </c>
+      <c r="D38" t="s">
+        <v>222</v>
+      </c>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>274</v>
+      </c>
+      <c r="C39" t="s">
+        <v>305</v>
+      </c>
+      <c r="D39" t="s">
+        <v>222</v>
+      </c>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>275</v>
+      </c>
+      <c r="C40" t="s">
+        <v>305</v>
+      </c>
+      <c r="D40" t="s">
+        <v>222</v>
+      </c>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>270</v>
+      </c>
+      <c r="C41" t="s">
+        <v>305</v>
+      </c>
+      <c r="D41" t="s">
+        <v>222</v>
+      </c>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" t="s">
+        <v>305</v>
+      </c>
+      <c r="D42" t="s">
+        <v>222</v>
+      </c>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" t="s">
+        <v>305</v>
+      </c>
+      <c r="D43" t="s">
+        <v>222</v>
+      </c>
+      <c r="E43" s="4"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>171</v>
+      </c>
+      <c r="C44" t="s">
+        <v>305</v>
+      </c>
+      <c r="D44" t="s">
+        <v>222</v>
+      </c>
+      <c r="E44" s="4"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" t="s">
+        <v>305</v>
+      </c>
+      <c r="D45" t="s">
+        <v>222</v>
+      </c>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" t="s">
+        <v>305</v>
+      </c>
+      <c r="D46" t="s">
+        <v>222</v>
+      </c>
+      <c r="E46" s="4"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>191</v>
+      </c>
+      <c r="C47" t="s">
+        <v>305</v>
+      </c>
+      <c r="D47" t="s">
+        <v>222</v>
+      </c>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" t="s">
+        <v>305</v>
+      </c>
+      <c r="D48" t="s">
+        <v>222</v>
+      </c>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>269</v>
+      </c>
+      <c r="C49" t="s">
+        <v>305</v>
+      </c>
+      <c r="D49" t="s">
+        <v>222</v>
+      </c>
+      <c r="E49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>156</v>
+      </c>
+      <c r="C50" t="s">
+        <v>305</v>
+      </c>
+      <c r="D50" t="s">
+        <v>222</v>
+      </c>
+      <c r="E50" s="4"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51" t="s">
+        <v>305</v>
+      </c>
+      <c r="D51" t="s">
+        <v>222</v>
+      </c>
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" t="s">
+        <v>305</v>
+      </c>
+      <c r="D52" t="s">
+        <v>222</v>
+      </c>
+      <c r="E52" s="4"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" t="s">
+        <v>305</v>
+      </c>
+      <c r="D53" t="s">
+        <v>222</v>
+      </c>
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" t="s">
+        <v>305</v>
+      </c>
+      <c r="D54" t="s">
+        <v>222</v>
+      </c>
+      <c r="E54" s="4"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>195</v>
+      </c>
+      <c r="C55" t="s">
+        <v>305</v>
+      </c>
+      <c r="D55" t="s">
+        <v>222</v>
+      </c>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>72</v>
+      </c>
+      <c r="C56" t="s">
+        <v>305</v>
+      </c>
+      <c r="D56" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>176</v>
+      </c>
+      <c r="C57" t="s">
+        <v>305</v>
+      </c>
+      <c r="D57" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>285</v>
+      </c>
+      <c r="C58" t="s">
+        <v>305</v>
+      </c>
+      <c r="D58" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>272</v>
+      </c>
+      <c r="C59" t="s">
+        <v>305</v>
+      </c>
+      <c r="D59" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>187</v>
+      </c>
+      <c r="C60" t="s">
+        <v>305</v>
+      </c>
+      <c r="D60" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>276</v>
+      </c>
+      <c r="C61" t="s">
+        <v>305</v>
+      </c>
+      <c r="D61" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>287</v>
+      </c>
+      <c r="C62" t="s">
+        <v>305</v>
+      </c>
+      <c r="D62" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" t="s">
+        <v>305</v>
+      </c>
+      <c r="D63" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>86</v>
+      </c>
+      <c r="C64" t="s">
+        <v>305</v>
+      </c>
+      <c r="D64" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>182</v>
+      </c>
+      <c r="C65" t="s">
+        <v>305</v>
+      </c>
+      <c r="D65" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>289</v>
+      </c>
+      <c r="C66" t="s">
+        <v>305</v>
+      </c>
+      <c r="D66" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>175</v>
+      </c>
+      <c r="C67" t="s">
+        <v>305</v>
+      </c>
+      <c r="D67" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>93</v>
+      </c>
+      <c r="C68" t="s">
+        <v>305</v>
+      </c>
+      <c r="D68" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>277</v>
+      </c>
+      <c r="C69" t="s">
+        <v>305</v>
+      </c>
+      <c r="D69" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>190</v>
+      </c>
+      <c r="C70" t="s">
+        <v>305</v>
+      </c>
+      <c r="D70" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>271</v>
+      </c>
+      <c r="C71" t="s">
+        <v>305</v>
+      </c>
+      <c r="D71" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>163</v>
+      </c>
+      <c r="C72" t="s">
+        <v>305</v>
+      </c>
+      <c r="D72" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>278</v>
+      </c>
+      <c r="C73" t="s">
+        <v>305</v>
+      </c>
+      <c r="D73" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>183</v>
+      </c>
+      <c r="C74" t="s">
+        <v>305</v>
+      </c>
+      <c r="D74" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>170</v>
+      </c>
+      <c r="C75" t="s">
+        <v>305</v>
+      </c>
+      <c r="D75" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>101</v>
+      </c>
+      <c r="C76" t="s">
+        <v>305</v>
+      </c>
+      <c r="D76" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>288</v>
+      </c>
+      <c r="C77" t="s">
+        <v>305</v>
+      </c>
+      <c r="D77" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>188</v>
+      </c>
+      <c r="C78" t="s">
+        <v>305</v>
+      </c>
+      <c r="D78" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>178</v>
+      </c>
+      <c r="C79" t="s">
+        <v>305</v>
+      </c>
+      <c r="D79" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>173</v>
+      </c>
+      <c r="C80" t="s">
+        <v>305</v>
+      </c>
+      <c r="D80" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>160</v>
+      </c>
+      <c r="C81" t="s">
+        <v>305</v>
+      </c>
+      <c r="D81" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>154</v>
+      </c>
+      <c r="C82" t="s">
+        <v>305</v>
+      </c>
+      <c r="D82" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>161</v>
+      </c>
+      <c r="C83" t="s">
+        <v>305</v>
+      </c>
+      <c r="D83" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F185"/>
   <sheetViews>
@@ -4935,77 +5310,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>